<commit_message>
para entrega 2a fase.
</commit_message>
<xml_diff>
--- a/Dados.xlsx
+++ b/Dados.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100">
   <si>
     <t>ID</t>
   </si>
@@ -28,7 +28,7 @@
     <t>VU</t>
   </si>
   <si>
-    <t>BR282</t>
+    <t>Geral</t>
   </si>
   <si>
     <t>topografia</t>
@@ -37,6 +37,9 @@
     <t>pavimentacao</t>
   </si>
   <si>
+    <t>pavimentado</t>
+  </si>
+  <si>
     <t>situacao</t>
   </si>
   <si>
@@ -49,51 +52,51 @@
     <t>LT_01</t>
   </si>
   <si>
+    <t>sim</t>
+  </si>
+  <si>
+    <t>plano</t>
+  </si>
+  <si>
+    <t>asfalto</t>
+  </si>
+  <si>
+    <t>esquina</t>
+  </si>
+  <si>
+    <t>Sorria Imoveis</t>
+  </si>
+  <si>
+    <t>http://www.sorriaimoveis.com.br/ImovelSelecionado.aspx?id=34294&amp;emp=27&amp;fin=1&amp;tit=terreno-codigo-2466-a-venda-no-bairro-centro-na-cidade-de-santo-amaro-da-imperatriz-condominio-</t>
+  </si>
+  <si>
+    <t>LT_02</t>
+  </si>
+  <si>
+    <t>meio</t>
+  </si>
+  <si>
+    <t>http://www.sorriaimoveis.com.br/ImovelSelecionado.aspx?id=35847&amp;emp=27&amp;fin=1&amp;tit=terreno-codigo-2671-a-venda-no-bairro-centro-na-cidade-de-santo-amaro-da-imperatriz-condominio-</t>
+  </si>
+  <si>
+    <t>LT_03</t>
+  </si>
+  <si>
+    <t>acidentado</t>
+  </si>
+  <si>
+    <t>CK Imoveis</t>
+  </si>
+  <si>
+    <t>http://www.ckimoveis.com.br/lotes/lote-16/index.htm</t>
+  </si>
+  <si>
+    <t>LT_04</t>
+  </si>
+  <si>
     <t>nao</t>
   </si>
   <si>
-    <t>plano</t>
-  </si>
-  <si>
-    <t>asfalto</t>
-  </si>
-  <si>
-    <t>esquina</t>
-  </si>
-  <si>
-    <t>Sorria Imoveis</t>
-  </si>
-  <si>
-    <t>http://www.sorriaimoveis.com.br/ImovelSelecionado.aspx?id=34294&amp;emp=27&amp;fin=1&amp;tit=terreno-codigo-2466-a-venda-no-bairro-centro-na-cidade-de-santo-amaro-da-imperatriz-condominio-</t>
-  </si>
-  <si>
-    <t>LT_02</t>
-  </si>
-  <si>
-    <t>meio</t>
-  </si>
-  <si>
-    <t>http://www.sorriaimoveis.com.br/ImovelSelecionado.aspx?id=35847&amp;emp=27&amp;fin=1&amp;tit=terreno-codigo-2671-a-venda-no-bairro-centro-na-cidade-de-santo-amaro-da-imperatriz-condominio-</t>
-  </si>
-  <si>
-    <t>LT_03</t>
-  </si>
-  <si>
-    <t>sim</t>
-  </si>
-  <si>
-    <t>acidentado</t>
-  </si>
-  <si>
-    <t>CK Imoveis</t>
-  </si>
-  <si>
-    <t>http://www.ckimoveis.com.br/lotes/lote-16/index.htm</t>
-  </si>
-  <si>
-    <t>LT_04</t>
-  </si>
-  <si>
     <t>http://www.sorriaimoveis.com.br/ImovelSelecionado.aspx?id=38885&amp;emp=27&amp;fin=1&amp;tit=terreno-codigo-2955-a-venda-no-bairro-centro-na-cidade-de-santo-amaro-da-imperatriz-condominio-</t>
   </si>
   <si>
@@ -299,6 +302,18 @@
   </si>
   <si>
     <t>http://www.ckimoveis.com.br/lotes/lote-09/index.htm</t>
+  </si>
+  <si>
+    <t>AVAL_1</t>
+  </si>
+  <si>
+    <t>AVAL_2</t>
+  </si>
+  <si>
+    <t>AVAL_3</t>
+  </si>
+  <si>
+    <t>AVAL_4</t>
   </si>
 </sst>
 </file>
@@ -306,14 +321,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="178" formatCode="0.00_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -322,16 +337,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FFCCCCCC"/>
+      <name val="Lucida Console"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -344,9 +358,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -360,11 +373,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -384,7 +397,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -399,14 +412,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -415,6 +421,29 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -443,6 +472,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -450,21 +486,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -475,31 +496,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -511,61 +664,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -578,84 +677,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -666,39 +687,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -713,15 +701,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -758,6 +737,15 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -766,6 +754,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -777,146 +798,146 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -929,7 +950,10 @@
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="11" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="11" applyFont="1" applyAlignment="1">
       <alignment horizontal="distributed" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1251,10 +1275,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J37"/>
+  <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1262,12 +1286,12 @@
     <col min="2" max="2" width="9.57142857142857"/>
     <col min="3" max="3" width="14.1428571428571"/>
     <col min="4" max="6" width="12.8571428571429"/>
-    <col min="7" max="8" width="14.4285714285714" customWidth="1"/>
-    <col min="9" max="9" width="14.7142857142857" customWidth="1"/>
-    <col min="10" max="10" width="106.390476190476" style="1" customWidth="1"/>
+    <col min="7" max="9" width="14.4285714285714" customWidth="1"/>
+    <col min="10" max="10" width="14.7142857142857" customWidth="1"/>
+    <col min="11" max="11" width="106.390476190476" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1295,13 +1319,16 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" ht="30" spans="1:10">
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" ht="30" spans="1:11">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B2" s="2">
         <v>28750</v>
@@ -1310,62 +1337,70 @@
         <v>3800000</v>
       </c>
       <c r="D2" s="3">
-        <f>C2/B2</f>
+        <f t="shared" ref="D2:D11" si="0">C2/B2</f>
         <v>132.173913043478</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" ht="30" spans="1:10">
+      <c r="K2" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" ht="30" spans="1:11">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B3" s="2">
         <v>1800</v>
       </c>
-      <c r="C3" s="3"/>
+      <c r="C3" s="3">
+        <v>2700000</v>
+      </c>
       <c r="D3" s="3">
-        <f>C3/B3</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1500</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
+        <v>19</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B4" s="2">
         <v>5373.72</v>
@@ -1374,29 +1409,32 @@
         <v>250000</v>
       </c>
       <c r="D4" s="3">
-        <f>C4/B4</f>
+        <f t="shared" si="0"/>
         <v>46.5227068027363</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="I4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="K4" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" ht="30" spans="1:10">
+    <row r="5" ht="30" spans="1:11">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -1407,31 +1445,34 @@
         <v>880000</v>
       </c>
       <c r="D5" s="3">
-        <f>C5/B5</f>
+        <f t="shared" si="0"/>
         <v>142.210730446025</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" ht="30" spans="1:10">
+        <v>19</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" ht="30" spans="1:11">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B6" s="2">
         <v>941</v>
@@ -1440,31 +1481,34 @@
         <v>800000</v>
       </c>
       <c r="D6" s="3">
-        <f>C6/B6</f>
+        <f t="shared" si="0"/>
         <v>850.159404888417</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" ht="30" spans="1:10">
+        <v>19</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" ht="30" spans="1:11">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B7" s="2">
         <v>838.72</v>
@@ -1473,31 +1517,34 @@
         <v>850000</v>
       </c>
       <c r="D7" s="3">
-        <f>C7/B7</f>
+        <f t="shared" si="0"/>
         <v>1013.44906524227</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="J7" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" ht="30" spans="1:10">
+      <c r="J7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" ht="30" spans="1:11">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B8" s="2">
         <v>777</v>
@@ -1506,31 +1553,34 @@
         <v>690000</v>
       </c>
       <c r="D8" s="3">
-        <f>C8/B8</f>
+        <f t="shared" si="0"/>
         <v>888.030888030888</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" ht="30" spans="1:10">
+        <v>19</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" ht="30" spans="1:11">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B9" s="2">
         <v>630</v>
@@ -1539,31 +1589,34 @@
         <v>600000</v>
       </c>
       <c r="D9" s="3">
-        <f>C9/B9</f>
+        <f t="shared" si="0"/>
         <v>952.380952380952</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I9" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="J9" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" ht="30" spans="1:10">
+      <c r="J9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" ht="30" spans="1:11">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B10" s="2">
         <v>1740</v>
@@ -1572,31 +1625,34 @@
         <v>380000</v>
       </c>
       <c r="D10" s="3">
-        <f>C10/B10</f>
+        <f t="shared" si="0"/>
         <v>218.390804597701</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J10" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" ht="30" spans="1:10">
+        <v>19</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K10" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" ht="30" spans="1:11">
       <c r="A11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B11" s="2">
         <v>7916.1</v>
@@ -1605,31 +1661,34 @@
         <v>360000</v>
       </c>
       <c r="D11" s="3">
-        <f>C11/B11</f>
+        <f t="shared" si="0"/>
         <v>45.4769394019782</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J11" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" ht="30" spans="1:10">
+        <v>19</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" ht="30" spans="1:11">
       <c r="A12" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B12" s="2">
         <v>585</v>
@@ -1638,31 +1697,34 @@
         <v>240000</v>
       </c>
       <c r="D12" s="3">
-        <f t="shared" ref="D12:D39" si="0">C12/B12</f>
+        <f t="shared" ref="D12:D39" si="1">C12/B12</f>
         <v>410.25641025641</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I12" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="J12" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" ht="30" spans="1:10">
+      <c r="J12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" ht="30" spans="1:11">
       <c r="A13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B13" s="2">
         <v>668.29</v>
@@ -1671,31 +1733,34 @@
         <v>230000</v>
       </c>
       <c r="D13" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>344.161965613731</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J13" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" ht="30" spans="1:10">
+        <v>19</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K13" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" ht="30" spans="1:11">
       <c r="A14" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B14" s="2">
         <v>3521.97</v>
@@ -1704,31 +1769,34 @@
         <v>300000</v>
       </c>
       <c r="D14" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>85.1796011891072</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J14" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" ht="30" spans="1:10">
+        <v>19</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K14" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" ht="30" spans="1:11">
       <c r="A15" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B15" s="2">
         <v>542.47</v>
@@ -1737,31 +1805,34 @@
         <v>200000</v>
       </c>
       <c r="D15" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>368.683982524379</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J15" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="16" ht="30" spans="1:10">
+        <v>19</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K15" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" ht="30" spans="1:11">
       <c r="A16" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B16" s="2">
         <v>700</v>
@@ -1770,31 +1841,34 @@
         <v>150000</v>
       </c>
       <c r="D16" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>214.285714285714</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J16" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="17" ht="30" spans="1:10">
+        <v>19</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K16" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" ht="30" spans="1:11">
       <c r="A17" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B17" s="2">
         <v>360</v>
@@ -1803,31 +1877,34 @@
         <v>130000</v>
       </c>
       <c r="D17" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>361.111111111111</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J17" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="18" ht="30" spans="1:10">
+        <v>19</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K17" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" ht="30" spans="1:11">
       <c r="A18" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B18" s="2">
         <v>364</v>
@@ -1836,31 +1913,34 @@
         <v>125000</v>
       </c>
       <c r="D18" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>343.406593406593</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J18" s="4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="19" ht="30" spans="1:10">
+        <v>19</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K18" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" ht="30" spans="1:11">
       <c r="A19" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B19" s="2">
         <v>364</v>
@@ -1869,31 +1949,34 @@
         <v>120000</v>
       </c>
       <c r="D19" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>329.67032967033</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J19" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="20" ht="30" spans="1:10">
+        <v>19</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K19" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" ht="30" spans="1:11">
       <c r="A20" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B20" s="2">
         <v>468</v>
@@ -1902,31 +1985,34 @@
         <v>120000</v>
       </c>
       <c r="D20" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>256.410256410256</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J20" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="21" ht="30" spans="1:10">
+        <v>19</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K20" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" ht="30" spans="1:11">
       <c r="A21" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B21" s="2">
         <v>328.77</v>
@@ -1935,31 +2021,34 @@
         <v>100000</v>
       </c>
       <c r="D21" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>304.164005231621</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J21" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="22" ht="30" spans="1:10">
+        <v>19</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K21" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" ht="30" spans="1:11">
       <c r="A22" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B22" s="2">
         <v>385</v>
@@ -1968,31 +2057,34 @@
         <v>95000</v>
       </c>
       <c r="D22" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>246.753246753247</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J22" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="23" ht="30" spans="1:10">
+        <v>19</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K22" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" ht="30" spans="1:11">
       <c r="A23" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B23" s="2">
         <v>1200</v>
@@ -2001,31 +2093,34 @@
         <v>90000</v>
       </c>
       <c r="D23" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>75</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J23" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="24" ht="30" spans="1:10">
+        <v>19</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K23" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" ht="30" spans="1:11">
       <c r="A24" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B24" s="2">
         <v>403</v>
@@ -2034,31 +2129,34 @@
         <v>80000</v>
       </c>
       <c r="D24" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>198.511166253102</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J24" s="4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="25" ht="30" spans="1:10">
+        <v>19</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K24" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" ht="30" spans="1:11">
       <c r="A25" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B25" s="2">
         <v>516</v>
@@ -2067,31 +2165,34 @@
         <v>60000</v>
       </c>
       <c r="D25" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>116.279069767442</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="F25" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J25" s="4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10">
+        <v>19</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K25" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
       <c r="A26" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B26">
         <v>472</v>
@@ -2100,31 +2201,34 @@
         <v>380000</v>
       </c>
       <c r="D26" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>805.084745762712</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="I26" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J26" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="J26" s="4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10">
+      <c r="K26" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
       <c r="A27" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B27">
         <v>380</v>
@@ -2133,31 +2237,34 @@
         <v>285000</v>
       </c>
       <c r="D27" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>750</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="I27" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J27" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="J27" s="4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10">
+      <c r="K27" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
       <c r="A28" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B28">
         <v>1030.49</v>
@@ -2166,31 +2273,34 @@
         <v>290000</v>
       </c>
       <c r="D28" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>281.419518869664</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="F28" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="I28" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J28" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="J28" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="29" ht="30" spans="1:10">
+      <c r="K28" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="29" ht="30" spans="1:11">
       <c r="A29" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B29">
         <v>2261</v>
@@ -2199,31 +2309,34 @@
         <v>398000</v>
       </c>
       <c r="D29" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>176.028306059266</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="J29" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J29" s="3" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="30" ht="30" spans="1:10">
+      <c r="K29" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="30" ht="30" spans="1:11">
       <c r="A30" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B30">
         <v>30000</v>
@@ -2232,31 +2345,34 @@
         <v>850000</v>
       </c>
       <c r="D30" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>28.3333333333333</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="J30" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="31" ht="30" spans="1:10">
+        <v>19</v>
+      </c>
+      <c r="J30" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="K30" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="31" ht="30" spans="1:11">
       <c r="A31" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B31">
         <v>360</v>
@@ -2265,31 +2381,34 @@
         <v>180000</v>
       </c>
       <c r="D31" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>500</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="J31" s="4" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="32" ht="30" spans="1:10">
+        <v>19</v>
+      </c>
+      <c r="J31" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="K31" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="32" ht="30" spans="1:11">
       <c r="A32" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B32">
         <v>384</v>
@@ -2298,31 +2417,34 @@
         <v>95000</v>
       </c>
       <c r="D32" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>247.395833333333</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="F32" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I32" t="s">
-        <v>76</v>
-      </c>
-      <c r="J32" s="4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="33" ht="30" spans="1:10">
+        <v>12</v>
+      </c>
+      <c r="I32" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J32" t="s">
+        <v>77</v>
+      </c>
+      <c r="K32" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="33" ht="30" spans="1:11">
       <c r="A33" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B33">
         <v>2000</v>
@@ -2331,31 +2453,34 @@
         <v>2000000</v>
       </c>
       <c r="D33" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1000</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I33" t="s">
-        <v>85</v>
-      </c>
-      <c r="J33" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I33" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J33" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="34" spans="1:10">
+      <c r="K33" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
       <c r="A34" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B34">
         <v>360</v>
@@ -2364,31 +2489,34 @@
         <v>105000</v>
       </c>
       <c r="D34" s="3">
-        <f>C34/B34</f>
+        <f t="shared" si="1"/>
         <v>291.666666666667</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I34" t="s">
+        <v>12</v>
+      </c>
+      <c r="I34" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J34" t="s">
         <v>23</v>
       </c>
-      <c r="J34" s="4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10">
+      <c r="K34" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
       <c r="A35" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B35">
         <v>400</v>
@@ -2397,31 +2525,34 @@
         <v>380000</v>
       </c>
       <c r="D35" s="3">
-        <f>C35/B35</f>
+        <f t="shared" si="1"/>
         <v>950</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I35" t="s">
+        <v>12</v>
+      </c>
+      <c r="I35" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J35" t="s">
         <v>23</v>
       </c>
-      <c r="J35" s="4" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10">
+      <c r="K35" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11">
       <c r="A36" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B36">
         <v>1507.17</v>
@@ -2430,31 +2561,34 @@
         <v>420000</v>
       </c>
       <c r="D36" s="3">
-        <f>C36/B36</f>
+        <f t="shared" si="1"/>
         <v>278.66796711718</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I36" t="s">
+        <v>26</v>
+      </c>
+      <c r="I36" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J36" t="s">
         <v>23</v>
       </c>
-      <c r="J36" s="4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10">
+      <c r="K36" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11">
       <c r="A37" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B37">
         <v>808.92</v>
@@ -2463,66 +2597,125 @@
         <v>370000</v>
       </c>
       <c r="D37" s="3">
-        <f>C37/B37</f>
+        <f t="shared" si="1"/>
         <v>457.39999011027</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="F37" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G37" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I37" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J37" t="s">
+        <v>23</v>
+      </c>
+      <c r="K37" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" t="s">
+        <v>96</v>
+      </c>
+      <c r="B38">
+        <v>360</v>
+      </c>
+      <c r="E38" t="s">
+        <v>12</v>
+      </c>
+      <c r="F38" t="s">
         <v>13</v>
       </c>
-      <c r="H37" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I37" t="s">
-        <v>23</v>
-      </c>
-      <c r="J37" s="4" t="s">
-        <v>94</v>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" t="s">
+        <v>97</v>
+      </c>
+      <c r="B39" s="4">
+        <v>360</v>
+      </c>
+      <c r="E39" t="s">
+        <v>12</v>
+      </c>
+      <c r="F39" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" t="s">
+        <v>98</v>
+      </c>
+      <c r="B40">
+        <v>360</v>
+      </c>
+      <c r="E40" t="s">
+        <v>26</v>
+      </c>
+      <c r="F40" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" t="s">
+        <v>99</v>
+      </c>
+      <c r="B41">
+        <v>360</v>
+      </c>
+      <c r="E41" t="s">
+        <v>26</v>
+      </c>
+      <c r="F41" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J31" r:id="rId1" display="https://www.vivareal.com.br/imovel/lote-terreno-centro-bairros-santo-amaro-da-imperatriz-360m2-venda-RS180000-id-93039881/?__vt=ranking:sem"/>
-    <hyperlink ref="J30" r:id="rId2" display="https://www.vivareal.com.br/imovel/lote-terreno-1-quartos-centro-bairros-santo-amaro-da-imperatriz-30000m2-venda-RS850000-id-87064814/?__vt=ranking:sem"/>
-    <hyperlink ref="J28" r:id="rId3" display="http://www.ckimoveis.com.br/lotes/lote-21/index.htm"/>
-    <hyperlink ref="J27" r:id="rId4" display="http://www.ckimoveis.com.br/lotes/lote-12/index.htm"/>
-    <hyperlink ref="J26" r:id="rId5" display="http://www.ckimoveis.com.br/lotes/lote-03/index.htm"/>
-    <hyperlink ref="J25" r:id="rId6" display="http://www.sorriaimoveis.com.br/ImovelSelecionado.aspx?id=53466&amp;emp=27&amp;fin=1&amp;tit=terreno-codigo-3796-a-venda-no-bairro-centro-na-cidade-de-santo-amaro-da-imperatriz-condominio-" tooltip="http://www.sorriaimoveis.com.br/ImovelSelecionado.aspx?id=53466&amp;emp=27&amp;fin=1&amp;tit=terreno-codigo-3796-a-venda-no-bairro-centro-na-cidade-de-santo-amaro-da-imperatriz-condominio-"/>
-    <hyperlink ref="J24" r:id="rId7" display="http://www.sorriaimoveis.com.br/ImovelSelecionado.aspx?id=47018&amp;emp=27&amp;fin=1&amp;tit=terreno-codigo-3224-a-venda-no-bairro-centro-na-cidade-de-santo-amaro-da-imperatriz-condominio-" tooltip="http://www.sorriaimoveis.com.br/ImovelSelecionado.aspx?id=47018&amp;emp=27&amp;fin=1&amp;tit=terreno-codigo-3224-a-venda-no-bairro-centro-na-cidade-de-santo-amaro-da-imperatriz-condominio-"/>
-    <hyperlink ref="J23" r:id="rId8" display="http://www.sorriaimoveis.com.br/ImovelSelecionado.aspx?id=52569&amp;emp=27&amp;fin=1&amp;tit=terreno-codigo-3680-a-venda-no-bairro-centro-na-cidade-de-santo-amaro-da-imperatriz-condominio-" tooltip="http://www.sorriaimoveis.com.br/ImovelSelecionado.aspx?id=52569&amp;emp=27&amp;fin=1&amp;tit=terreno-codigo-3680-a-venda-no-bairro-centro-na-cidade-de-santo-amaro-da-imperatriz-condominio-"/>
-    <hyperlink ref="J22" r:id="rId9" display="http://www.sorriaimoveis.com.br/ImovelSelecionado.aspx?id=35593&amp;emp=27&amp;fin=1&amp;tit=terreno-codigo-2626-a-venda-no-bairro-centro-na-cidade-de-santo-amaro-da-imperatriz-condominio-"/>
-    <hyperlink ref="J21" r:id="rId10" display="http://www.sorriaimoveis.com.br/ImovelSelecionado.aspx?id=51914&amp;emp=27&amp;fin=1&amp;tit=terreno-codigo-3572-a-venda-no-bairro-centro-na-cidade-de-santo-amaro-da-imperatriz-condominio-"/>
-    <hyperlink ref="J20" r:id="rId11" display="http://www.sorriaimoveis.com.br/ImovelSelecionado.aspx?id=52951&amp;emp=27&amp;fin=1&amp;tit=terreno-codigo-3730-a-venda-no-bairro-centro-na-cidade-de-santo-amaro-da-imperatriz-condominio-"/>
-    <hyperlink ref="J19" r:id="rId12" display="http://www.sorriaimoveis.com.br/ImovelSelecionado.aspx?id=50437&amp;emp=27&amp;fin=1&amp;tit=terreno-codigo-3435-a-venda-no-bairro-centro-na-cidade-de-santo-amaro-da-imperatriz-condominio-"/>
-    <hyperlink ref="J18" r:id="rId13" display="http://www.sorriaimoveis.com.br/ImovelSelecionado.aspx?id=52273&amp;emp=27&amp;fin=1&amp;tit=terreno-codigo-3634-a-venda-no-bairro-centro-na-cidade-de-santo-amaro-da-imperatriz-condominio-"/>
-    <hyperlink ref="J17" r:id="rId14" display="http://www.sorriaimoveis.com.br/ImovelSelecionado.aspx?id=38442&amp;emp=27&amp;fin=1&amp;tit=terreno-codigo-2919-a-venda-no-bairro-centro-na-cidade-de-santo-amaro-da-imperatriz-condominio-loteamento-estefano-becker"/>
-    <hyperlink ref="J16" r:id="rId15" display="http://www.sorriaimoveis.com.br/ImovelSelecionado.aspx?id=22320&amp;emp=27&amp;fin=1&amp;tit=terreno-codigo-1541-a-venda-no-bairro-centro-na-cidade-de-santo-amaro-da-imperatriz-condominio-"/>
-    <hyperlink ref="J15" r:id="rId16" display="http://www.sorriaimoveis.com.br/ImovelSelecionado.aspx?id=53500&amp;emp=27&amp;fin=1&amp;tit=terreno-codigo-3803-a-venda-no-bairro-centro-na-cidade-de-santo-amaro-da-imperatriz-condominio-"/>
-    <hyperlink ref="J14" r:id="rId17" display="http://www.sorriaimoveis.com.br/ImovelSelecionado.aspx?id=54031&amp;emp=27&amp;fin=1&amp;tit=terreno-codigo-3872-a-venda-no-bairro-centro-na-cidade-de-santo-amaro-da-imperatriz-condominio-"/>
-    <hyperlink ref="J13" r:id="rId18" display="http://www.sorriaimoveis.com.br/ImovelSelecionado.aspx?id=51345&amp;emp=27&amp;fin=1&amp;tit=terreno-codigo-3497-a-venda-no-bairro-centro-na-cidade-de-santo-amaro-da-imperatriz-condominio-loteamento-estefano-becker"/>
-    <hyperlink ref="J12" r:id="rId19" display="http://www.sorriaimoveis.com.br/ImovelSelecionado.aspx?id=52529&amp;emp=27&amp;fin=1&amp;tit=terreno-codigo-3675-a-venda-no-bairro-centro-na-cidade-de-santo-amaro-da-imperatriz-condominio-"/>
-    <hyperlink ref="J11" r:id="rId20" display="http://www.sorriaimoveis.com.br/ImovelSelecionado.aspx?id=26000&amp;emp=27&amp;fin=1&amp;tit=terreno-codigo-1891-a-venda-no-bairro-centro-na-cidade-de-santo-amaro-da-imperatriz-condominio-"/>
-    <hyperlink ref="J10" r:id="rId21" display="http://www.sorriaimoveis.com.br/ImovelSelecionado.aspx?id=46549&amp;emp=27&amp;fin=1&amp;tit=terreno-codigo-3186-a-venda-no-bairro-centro-na-cidade-de-santo-amaro-da-imperatriz-condominio-"/>
-    <hyperlink ref="J9" r:id="rId22" display="http://www.sorriaimoveis.com.br/ImovelSelecionado.aspx?id=53817&amp;emp=27&amp;fin=1&amp;tit=terreno-codigo-3838-a-venda-no-bairro-centro-na-cidade-de-santo-amaro-da-imperatriz-condominio-"/>
-    <hyperlink ref="J8" r:id="rId23" display="http://www.sorriaimoveis.com.br/ImovelSelecionado.aspx?id=26841&amp;emp=27&amp;fin=1&amp;tit=terreno-codigo-2015-a-venda-no-bairro-centro-na-cidade-de-santo-amaro-da-imperatriz-condominio-"/>
-    <hyperlink ref="J7" r:id="rId24" display="http://www.sorriaimoveis.com.br/ImovelSelecionado.aspx?id=34324&amp;emp=27&amp;fin=1&amp;tit=terreno-codigo-2477-a-venda-no-bairro-centro-na-cidade-de-santo-amaro-da-imperatriz-condominio-"/>
-    <hyperlink ref="J6" r:id="rId25" display="http://www.sorriaimoveis.com.br/ImovelSelecionado.aspx?id=37614&amp;emp=27&amp;fin=1&amp;tit=terreno-codigo-2837-a-venda-no-bairro-centro-na-cidade-de-santo-amaro-da-imperatriz-condominio-"/>
-    <hyperlink ref="J5" r:id="rId26" display="http://www.sorriaimoveis.com.br/ImovelSelecionado.aspx?id=38885&amp;emp=27&amp;fin=1&amp;tit=terreno-codigo-2955-a-venda-no-bairro-centro-na-cidade-de-santo-amaro-da-imperatriz-condominio-"/>
-    <hyperlink ref="J3" r:id="rId27" display="http://www.sorriaimoveis.com.br/ImovelSelecionado.aspx?id=35847&amp;emp=27&amp;fin=1&amp;tit=terreno-codigo-2671-a-venda-no-bairro-centro-na-cidade-de-santo-amaro-da-imperatriz-condominio-"/>
-    <hyperlink ref="J2" r:id="rId28" display="http://www.sorriaimoveis.com.br/ImovelSelecionado.aspx?id=34294&amp;emp=27&amp;fin=1&amp;tit=terreno-codigo-2466-a-venda-no-bairro-centro-na-cidade-de-santo-amaro-da-imperatriz-condominio-"/>
-    <hyperlink ref="J29" r:id="rId29" display="https://www.vivareal.com.br/imovel/lote-terreno-centro-bairros-santo-amaro-da-imperatriz-2261m2-venda-RS398000-id-81633663/?__vt=ranking:sem"/>
-    <hyperlink ref="J32" r:id="rId30" display="https://www.vivareal.com.br/imovel/lote-terreno-sao-francisco-bairros-santo-amaro-da-imperatriz-384m2-venda-RS95000-id-95330494/?__vt=ranking:default"/>
-    <hyperlink ref="J33" r:id="rId31" display="https://sc.olx.com.br/florianopolis-e-regiao/terrenos/terreno-4-000-m-area-nobre-santo-amaro-da-imperatriz-a-25-min-de-florianopolis-sc-510157698"/>
-    <hyperlink ref="J34" r:id="rId32" display="http://www.ckimoveis.com.br/lotes/lote-17/index.htm"/>
-    <hyperlink ref="J35" r:id="rId33" display="http://www.ckimoveis.com.br/lotes/lote-26/index.htm"/>
-    <hyperlink ref="J36" r:id="rId34" display="http://www.ckimoveis.com.br/lotes/lote-35/index.htm"/>
-    <hyperlink ref="J37" r:id="rId35" display="http://www.ckimoveis.com.br/lotes/lote-09/index.htm"/>
-    <hyperlink ref="J4" r:id="rId36" display="http://www.ckimoveis.com.br/lotes/lote-16/index.htm"/>
+    <hyperlink ref="K31" r:id="rId1" display="https://www.vivareal.com.br/imovel/lote-terreno-centro-bairros-santo-amaro-da-imperatriz-360m2-venda-RS180000-id-93039881/?__vt=ranking:sem"/>
+    <hyperlink ref="K30" r:id="rId2" display="https://www.vivareal.com.br/imovel/lote-terreno-1-quartos-centro-bairros-santo-amaro-da-imperatriz-30000m2-venda-RS850000-id-87064814/?__vt=ranking:sem"/>
+    <hyperlink ref="K28" r:id="rId3" display="http://www.ckimoveis.com.br/lotes/lote-21/index.htm"/>
+    <hyperlink ref="K27" r:id="rId4" display="http://www.ckimoveis.com.br/lotes/lote-12/index.htm"/>
+    <hyperlink ref="K26" r:id="rId5" display="http://www.ckimoveis.com.br/lotes/lote-03/index.htm"/>
+    <hyperlink ref="K25" r:id="rId6" display="http://www.sorriaimoveis.com.br/ImovelSelecionado.aspx?id=53466&amp;emp=27&amp;fin=1&amp;tit=terreno-codigo-3796-a-venda-no-bairro-centro-na-cidade-de-santo-amaro-da-imperatriz-condominio-" tooltip="http://www.sorriaimoveis.com.br/ImovelSelecionado.aspx?id=53466&amp;emp=27&amp;fin=1&amp;tit=terreno-codigo-3796-a-venda-no-bairro-centro-na-cidade-de-santo-amaro-da-imperatriz-condominio-"/>
+    <hyperlink ref="K24" r:id="rId7" display="http://www.sorriaimoveis.com.br/ImovelSelecionado.aspx?id=47018&amp;emp=27&amp;fin=1&amp;tit=terreno-codigo-3224-a-venda-no-bairro-centro-na-cidade-de-santo-amaro-da-imperatriz-condominio-" tooltip="http://www.sorriaimoveis.com.br/ImovelSelecionado.aspx?id=47018&amp;emp=27&amp;fin=1&amp;tit=terreno-codigo-3224-a-venda-no-bairro-centro-na-cidade-de-santo-amaro-da-imperatriz-condominio-"/>
+    <hyperlink ref="K23" r:id="rId8" display="http://www.sorriaimoveis.com.br/ImovelSelecionado.aspx?id=52569&amp;emp=27&amp;fin=1&amp;tit=terreno-codigo-3680-a-venda-no-bairro-centro-na-cidade-de-santo-amaro-da-imperatriz-condominio-" tooltip="http://www.sorriaimoveis.com.br/ImovelSelecionado.aspx?id=52569&amp;emp=27&amp;fin=1&amp;tit=terreno-codigo-3680-a-venda-no-bairro-centro-na-cidade-de-santo-amaro-da-imperatriz-condominio-"/>
+    <hyperlink ref="K22" r:id="rId9" display="http://www.sorriaimoveis.com.br/ImovelSelecionado.aspx?id=35593&amp;emp=27&amp;fin=1&amp;tit=terreno-codigo-2626-a-venda-no-bairro-centro-na-cidade-de-santo-amaro-da-imperatriz-condominio-"/>
+    <hyperlink ref="K21" r:id="rId10" display="http://www.sorriaimoveis.com.br/ImovelSelecionado.aspx?id=51914&amp;emp=27&amp;fin=1&amp;tit=terreno-codigo-3572-a-venda-no-bairro-centro-na-cidade-de-santo-amaro-da-imperatriz-condominio-"/>
+    <hyperlink ref="K20" r:id="rId11" display="http://www.sorriaimoveis.com.br/ImovelSelecionado.aspx?id=52951&amp;emp=27&amp;fin=1&amp;tit=terreno-codigo-3730-a-venda-no-bairro-centro-na-cidade-de-santo-amaro-da-imperatriz-condominio-"/>
+    <hyperlink ref="K19" r:id="rId12" display="http://www.sorriaimoveis.com.br/ImovelSelecionado.aspx?id=50437&amp;emp=27&amp;fin=1&amp;tit=terreno-codigo-3435-a-venda-no-bairro-centro-na-cidade-de-santo-amaro-da-imperatriz-condominio-"/>
+    <hyperlink ref="K18" r:id="rId13" display="http://www.sorriaimoveis.com.br/ImovelSelecionado.aspx?id=52273&amp;emp=27&amp;fin=1&amp;tit=terreno-codigo-3634-a-venda-no-bairro-centro-na-cidade-de-santo-amaro-da-imperatriz-condominio-"/>
+    <hyperlink ref="K17" r:id="rId14" display="http://www.sorriaimoveis.com.br/ImovelSelecionado.aspx?id=38442&amp;emp=27&amp;fin=1&amp;tit=terreno-codigo-2919-a-venda-no-bairro-centro-na-cidade-de-santo-amaro-da-imperatriz-condominio-loteamento-estefano-becker"/>
+    <hyperlink ref="K16" r:id="rId15" display="http://www.sorriaimoveis.com.br/ImovelSelecionado.aspx?id=22320&amp;emp=27&amp;fin=1&amp;tit=terreno-codigo-1541-a-venda-no-bairro-centro-na-cidade-de-santo-amaro-da-imperatriz-condominio-"/>
+    <hyperlink ref="K15" r:id="rId16" display="http://www.sorriaimoveis.com.br/ImovelSelecionado.aspx?id=53500&amp;emp=27&amp;fin=1&amp;tit=terreno-codigo-3803-a-venda-no-bairro-centro-na-cidade-de-santo-amaro-da-imperatriz-condominio-"/>
+    <hyperlink ref="K14" r:id="rId17" display="http://www.sorriaimoveis.com.br/ImovelSelecionado.aspx?id=54031&amp;emp=27&amp;fin=1&amp;tit=terreno-codigo-3872-a-venda-no-bairro-centro-na-cidade-de-santo-amaro-da-imperatriz-condominio-"/>
+    <hyperlink ref="K13" r:id="rId18" display="http://www.sorriaimoveis.com.br/ImovelSelecionado.aspx?id=51345&amp;emp=27&amp;fin=1&amp;tit=terreno-codigo-3497-a-venda-no-bairro-centro-na-cidade-de-santo-amaro-da-imperatriz-condominio-loteamento-estefano-becker"/>
+    <hyperlink ref="K12" r:id="rId19" display="http://www.sorriaimoveis.com.br/ImovelSelecionado.aspx?id=52529&amp;emp=27&amp;fin=1&amp;tit=terreno-codigo-3675-a-venda-no-bairro-centro-na-cidade-de-santo-amaro-da-imperatriz-condominio-"/>
+    <hyperlink ref="K11" r:id="rId20" display="http://www.sorriaimoveis.com.br/ImovelSelecionado.aspx?id=26000&amp;emp=27&amp;fin=1&amp;tit=terreno-codigo-1891-a-venda-no-bairro-centro-na-cidade-de-santo-amaro-da-imperatriz-condominio-"/>
+    <hyperlink ref="K10" r:id="rId21" display="http://www.sorriaimoveis.com.br/ImovelSelecionado.aspx?id=46549&amp;emp=27&amp;fin=1&amp;tit=terreno-codigo-3186-a-venda-no-bairro-centro-na-cidade-de-santo-amaro-da-imperatriz-condominio-"/>
+    <hyperlink ref="K9" r:id="rId22" display="http://www.sorriaimoveis.com.br/ImovelSelecionado.aspx?id=53817&amp;emp=27&amp;fin=1&amp;tit=terreno-codigo-3838-a-venda-no-bairro-centro-na-cidade-de-santo-amaro-da-imperatriz-condominio-"/>
+    <hyperlink ref="K8" r:id="rId23" display="http://www.sorriaimoveis.com.br/ImovelSelecionado.aspx?id=26841&amp;emp=27&amp;fin=1&amp;tit=terreno-codigo-2015-a-venda-no-bairro-centro-na-cidade-de-santo-amaro-da-imperatriz-condominio-"/>
+    <hyperlink ref="K7" r:id="rId24" display="http://www.sorriaimoveis.com.br/ImovelSelecionado.aspx?id=34324&amp;emp=27&amp;fin=1&amp;tit=terreno-codigo-2477-a-venda-no-bairro-centro-na-cidade-de-santo-amaro-da-imperatriz-condominio-"/>
+    <hyperlink ref="K6" r:id="rId25" display="http://www.sorriaimoveis.com.br/ImovelSelecionado.aspx?id=37614&amp;emp=27&amp;fin=1&amp;tit=terreno-codigo-2837-a-venda-no-bairro-centro-na-cidade-de-santo-amaro-da-imperatriz-condominio-"/>
+    <hyperlink ref="K5" r:id="rId26" display="http://www.sorriaimoveis.com.br/ImovelSelecionado.aspx?id=38885&amp;emp=27&amp;fin=1&amp;tit=terreno-codigo-2955-a-venda-no-bairro-centro-na-cidade-de-santo-amaro-da-imperatriz-condominio-"/>
+    <hyperlink ref="K3" r:id="rId27" display="http://www.sorriaimoveis.com.br/ImovelSelecionado.aspx?id=35847&amp;emp=27&amp;fin=1&amp;tit=terreno-codigo-2671-a-venda-no-bairro-centro-na-cidade-de-santo-amaro-da-imperatriz-condominio-"/>
+    <hyperlink ref="K2" r:id="rId28" display="http://www.sorriaimoveis.com.br/ImovelSelecionado.aspx?id=34294&amp;emp=27&amp;fin=1&amp;tit=terreno-codigo-2466-a-venda-no-bairro-centro-na-cidade-de-santo-amaro-da-imperatriz-condominio-"/>
+    <hyperlink ref="K29" r:id="rId29" display="https://www.vivareal.com.br/imovel/lote-terreno-centro-bairros-santo-amaro-da-imperatriz-2261m2-venda-RS398000-id-81633663/?__vt=ranking:sem"/>
+    <hyperlink ref="K32" r:id="rId30" display="https://www.vivareal.com.br/imovel/lote-terreno-sao-francisco-bairros-santo-amaro-da-imperatriz-384m2-venda-RS95000-id-95330494/?__vt=ranking:default"/>
+    <hyperlink ref="K33" r:id="rId31" display="https://sc.olx.com.br/florianopolis-e-regiao/terrenos/terreno-4-000-m-area-nobre-santo-amaro-da-imperatriz-a-25-min-de-florianopolis-sc-510157698"/>
+    <hyperlink ref="K34" r:id="rId32" display="http://www.ckimoveis.com.br/lotes/lote-17/index.htm"/>
+    <hyperlink ref="K35" r:id="rId33" display="http://www.ckimoveis.com.br/lotes/lote-26/index.htm"/>
+    <hyperlink ref="K36" r:id="rId34" display="http://www.ckimoveis.com.br/lotes/lote-35/index.htm"/>
+    <hyperlink ref="K37" r:id="rId35" display="http://www.ckimoveis.com.br/lotes/lote-09/index.htm"/>
+    <hyperlink ref="K4" r:id="rId36" display="http://www.ckimoveis.com.br/lotes/lote-16/index.htm"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>

</xml_diff>